<commit_message>
worked on information extraction
</commit_message>
<xml_diff>
--- a/data/annotated/Labels - https___doi.org_10.1093_ehr_ceab280.xlsx
+++ b/data/annotated/Labels - https___doi.org_10.1093_ehr_ceab280.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quenzer/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quenzer/Desktop/Data Science/3. Semester 2023 WS/Data Analysis Project/A-blessing-or-a-curse-Analysis-of-scholarly-citations/data/annotated/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C8AC64C-E513-F140-97EC-71E96582754E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3765B4A9-ACC6-E847-8A8A-394A47CD8B54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,9 +41,6 @@
     <t>Subset</t>
   </si>
   <si>
-    <t>Author/s</t>
-  </si>
-  <si>
     <t>Title</t>
   </si>
   <si>
@@ -603,6 +600,9 @@
   </si>
   <si>
     <t>Bond Men Made Free</t>
+  </si>
+  <si>
+    <t>Authors</t>
   </si>
 </sst>
 </file>
@@ -896,7 +896,7 @@
   <dimension ref="A1:G1004"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -913,18 +913,18 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" ht="15">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -933,7 +933,7 @@
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E2" s="2">
         <v>0</v>
@@ -949,10 +949,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="E3" s="2">
         <v>0</v>
@@ -960,7 +960,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" ht="15">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -983,10 +983,10 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="E5" s="2">
         <v>1</v>
@@ -1002,10 +1002,10 @@
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="E6" s="2">
         <v>1</v>
@@ -1021,10 +1021,10 @@
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="E7" s="2">
         <v>0</v>
@@ -1040,10 +1040,10 @@
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="E8" s="2">
         <v>0</v>
@@ -1059,10 +1059,10 @@
         <v>2</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="E9" s="2">
         <v>0</v>
@@ -1078,10 +1078,10 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="E10" s="2">
         <v>0</v>
@@ -1098,7 +1098,7 @@
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E11" s="2">
         <v>0</v>
@@ -1114,10 +1114,10 @@
         <v>1</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="E12" s="2">
         <v>1</v>
@@ -1133,10 +1133,10 @@
         <v>2</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="E13" s="2">
         <v>1</v>
@@ -1152,10 +1152,10 @@
         <v>3</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="E14" s="2">
         <v>1</v>
@@ -1171,10 +1171,10 @@
         <v>1</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="E15" s="2">
         <v>0</v>
@@ -1190,10 +1190,10 @@
         <v>1</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="E16" s="2">
         <v>0</v>
@@ -1209,10 +1209,10 @@
         <v>2</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E17" s="2">
         <v>0</v>
@@ -1228,10 +1228,10 @@
         <v>1</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="E18" s="2">
         <v>0</v>
@@ -1247,10 +1247,10 @@
         <v>1</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="E19" s="2">
         <v>0</v>
@@ -1266,10 +1266,10 @@
         <v>1</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="E20" s="2">
         <v>0</v>
@@ -1300,10 +1300,10 @@
         <v>1</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="E22" s="2">
         <v>0</v>
@@ -1334,10 +1334,10 @@
         <v>1</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="E24" s="2">
         <v>0</v>
@@ -1353,10 +1353,10 @@
         <v>1</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="E25" s="2">
         <v>0</v>
@@ -1387,10 +1387,10 @@
         <v>1</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E27" s="2">
         <v>0</v>
@@ -1406,10 +1406,10 @@
         <v>1</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="E28" s="2">
         <v>0</v>
@@ -1425,10 +1425,10 @@
         <v>1</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E29" s="2">
         <v>1</v>
@@ -1444,10 +1444,10 @@
         <v>1</v>
       </c>
       <c r="C30" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="E30" s="2">
         <v>0</v>
@@ -1463,10 +1463,10 @@
         <v>2</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="E31" s="2">
         <v>0</v>
@@ -1482,10 +1482,10 @@
         <v>3</v>
       </c>
       <c r="C32" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="E32" s="2">
         <v>0</v>
@@ -1501,10 +1501,10 @@
         <v>1</v>
       </c>
       <c r="C33" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="E33" s="2">
         <v>1</v>
@@ -1520,10 +1520,10 @@
         <v>1</v>
       </c>
       <c r="C34" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="E34" s="2">
         <v>0</v>
@@ -1539,10 +1539,10 @@
         <v>1</v>
       </c>
       <c r="C35" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="E35" s="2">
         <v>0</v>
@@ -1558,10 +1558,10 @@
         <v>1</v>
       </c>
       <c r="C36" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="E36" s="2">
         <v>0</v>
@@ -1577,10 +1577,10 @@
         <v>1</v>
       </c>
       <c r="C37" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="E37" s="2">
         <v>0</v>
@@ -1596,10 +1596,10 @@
         <v>1</v>
       </c>
       <c r="C38" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="E38" s="2">
         <v>0</v>
@@ -1615,10 +1615,10 @@
         <v>1</v>
       </c>
       <c r="C39" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="E39" s="2">
         <v>0</v>
@@ -1634,10 +1634,10 @@
         <v>1</v>
       </c>
       <c r="C40" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="E40" s="2">
         <v>0</v>
@@ -1653,10 +1653,10 @@
         <v>1</v>
       </c>
       <c r="C41" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="E41" s="2">
         <v>0</v>
@@ -1672,10 +1672,10 @@
         <v>1</v>
       </c>
       <c r="C42" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="E42" s="2">
         <v>0</v>
@@ -1691,10 +1691,10 @@
         <v>1</v>
       </c>
       <c r="C43" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="E43" s="2">
         <v>0</v>
@@ -1710,10 +1710,10 @@
         <v>1</v>
       </c>
       <c r="C44" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="E44" s="2">
         <v>0</v>
@@ -1729,10 +1729,10 @@
         <v>1</v>
       </c>
       <c r="C45" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="E45" s="2">
         <v>0</v>
@@ -1763,10 +1763,10 @@
         <v>1</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E47" s="2">
         <v>0</v>
@@ -1812,10 +1812,10 @@
         <v>2</v>
       </c>
       <c r="C50" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>78</v>
       </c>
       <c r="E50" s="2">
         <v>0</v>
@@ -1831,10 +1831,10 @@
         <v>1</v>
       </c>
       <c r="C51" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="E51" s="2">
         <v>0</v>
@@ -1850,10 +1850,10 @@
         <v>2</v>
       </c>
       <c r="C52" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="E52" s="2">
         <v>0</v>
@@ -1869,10 +1869,10 @@
         <v>1</v>
       </c>
       <c r="C53" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="E53" s="2">
         <v>0</v>
@@ -1888,10 +1888,10 @@
         <v>1</v>
       </c>
       <c r="C54" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="E54" s="2">
         <v>0</v>
@@ -1908,7 +1908,7 @@
       </c>
       <c r="C55" s="1"/>
       <c r="D55" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E55" s="2">
         <v>0</v>
@@ -1924,10 +1924,10 @@
         <v>1</v>
       </c>
       <c r="C56" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D56" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="D56" s="4" t="s">
-        <v>87</v>
       </c>
       <c r="E56" s="2">
         <v>0</v>
@@ -1943,10 +1943,10 @@
         <v>1</v>
       </c>
       <c r="C57" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="E57" s="2">
         <v>1</v>
@@ -1962,10 +1962,10 @@
         <v>1</v>
       </c>
       <c r="C58" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="E58" s="2">
         <v>0</v>
@@ -1981,10 +1981,10 @@
         <v>1</v>
       </c>
       <c r="C59" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="E59" s="2">
         <v>0</v>
@@ -2000,10 +2000,10 @@
         <v>1</v>
       </c>
       <c r="C60" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D60" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="E60" s="2">
         <v>0</v>
@@ -2019,10 +2019,10 @@
         <v>1</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E61" s="2">
         <v>1</v>
@@ -2038,10 +2038,10 @@
         <v>1</v>
       </c>
       <c r="C62" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="E62" s="2">
         <v>0</v>
@@ -2057,10 +2057,10 @@
         <v>1</v>
       </c>
       <c r="C63" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D63" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="E63" s="2">
         <v>0</v>
@@ -2076,10 +2076,10 @@
         <v>1</v>
       </c>
       <c r="C64" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D64" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="E64" s="2">
         <v>0</v>
@@ -2095,10 +2095,10 @@
         <v>1</v>
       </c>
       <c r="C65" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>100</v>
       </c>
       <c r="E65" s="2">
         <v>0</v>
@@ -2114,10 +2114,10 @@
         <v>1</v>
       </c>
       <c r="C66" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D66" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>100</v>
       </c>
       <c r="E66" s="2">
         <v>0</v>
@@ -2133,10 +2133,10 @@
         <v>1</v>
       </c>
       <c r="C67" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D67" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>102</v>
       </c>
       <c r="E67" s="2">
         <v>0</v>
@@ -2152,10 +2152,10 @@
         <v>1</v>
       </c>
       <c r="C68" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D68" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>104</v>
       </c>
       <c r="E68" s="2">
         <v>0</v>
@@ -2171,10 +2171,10 @@
         <v>2</v>
       </c>
       <c r="C69" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D69" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>106</v>
       </c>
       <c r="E69" s="2">
         <v>0</v>
@@ -2190,10 +2190,10 @@
         <v>3</v>
       </c>
       <c r="C70" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D70" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>108</v>
       </c>
       <c r="E70" s="2">
         <v>0</v>
@@ -2209,10 +2209,10 @@
         <v>4</v>
       </c>
       <c r="C71" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D71" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="E71" s="2">
         <v>0</v>
@@ -2228,10 +2228,10 @@
         <v>1</v>
       </c>
       <c r="C72" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D72" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>112</v>
       </c>
       <c r="E72" s="2">
         <v>0</v>
@@ -2247,10 +2247,10 @@
         <v>1</v>
       </c>
       <c r="C73" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D73" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>114</v>
       </c>
       <c r="E73" s="2">
         <v>0</v>
@@ -2266,10 +2266,10 @@
         <v>1</v>
       </c>
       <c r="C74" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D74" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>116</v>
       </c>
       <c r="E74" s="2">
         <v>0</v>
@@ -2285,10 +2285,10 @@
         <v>1</v>
       </c>
       <c r="C75" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D75" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>118</v>
       </c>
       <c r="E75" s="2">
         <v>0</v>
@@ -2304,10 +2304,10 @@
         <v>1</v>
       </c>
       <c r="C76" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D76" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>120</v>
       </c>
       <c r="E76" s="2">
         <v>0</v>
@@ -2323,10 +2323,10 @@
         <v>2</v>
       </c>
       <c r="C77" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D77" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>122</v>
       </c>
       <c r="E77" s="2">
         <v>0</v>
@@ -2342,10 +2342,10 @@
         <v>1</v>
       </c>
       <c r="C78" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D78" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>124</v>
       </c>
       <c r="E78" s="2">
         <v>0</v>
@@ -2361,10 +2361,10 @@
         <v>1</v>
       </c>
       <c r="C79" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D79" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="E79" s="2">
         <v>1</v>
@@ -2380,10 +2380,10 @@
         <v>1</v>
       </c>
       <c r="C80" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D80" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>126</v>
       </c>
       <c r="E80" s="2">
         <v>0</v>
@@ -2400,7 +2400,7 @@
       </c>
       <c r="C81" s="1"/>
       <c r="D81" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E81" s="2">
         <v>0</v>
@@ -2416,10 +2416,10 @@
         <v>1</v>
       </c>
       <c r="C82" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D82" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>129</v>
       </c>
       <c r="E82" s="2">
         <v>0</v>
@@ -2435,10 +2435,10 @@
         <v>1</v>
       </c>
       <c r="C83" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D83" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>131</v>
       </c>
       <c r="E83" s="2">
         <v>1</v>
@@ -2454,10 +2454,10 @@
         <v>1</v>
       </c>
       <c r="C84" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D84" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>133</v>
       </c>
       <c r="E84" s="2">
         <v>0</v>
@@ -2473,10 +2473,10 @@
         <v>1</v>
       </c>
       <c r="C85" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D85" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>135</v>
       </c>
       <c r="E85" s="2">
         <v>0</v>
@@ -2492,10 +2492,10 @@
         <v>1</v>
       </c>
       <c r="C86" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D86" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="E86" s="2">
         <v>0</v>
@@ -2511,10 +2511,10 @@
         <v>1</v>
       </c>
       <c r="C87" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D87" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>133</v>
       </c>
       <c r="E87" s="2">
         <v>0</v>
@@ -2530,10 +2530,10 @@
         <v>2</v>
       </c>
       <c r="C88" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D88" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>137</v>
       </c>
       <c r="E88" s="2">
         <v>0</v>
@@ -2549,7 +2549,7 @@
         <v>1</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E89" s="2">
         <v>0</v>
@@ -2565,10 +2565,10 @@
         <v>2</v>
       </c>
       <c r="C90" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D90" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>140</v>
       </c>
       <c r="E90" s="2">
         <v>0</v>
@@ -2584,7 +2584,7 @@
         <v>1</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D91" s="1"/>
       <c r="E91" s="2">
@@ -2601,7 +2601,7 @@
         <v>1</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D92" s="1"/>
       <c r="E92" s="2">
@@ -2618,7 +2618,7 @@
         <v>1</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D93" s="1"/>
       <c r="E93" s="2">
@@ -2635,7 +2635,7 @@
         <v>1</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D94" s="1"/>
       <c r="E94" s="2">
@@ -2652,7 +2652,7 @@
         <v>1</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D95" s="1"/>
       <c r="E95" s="2">
@@ -2669,7 +2669,7 @@
         <v>1</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D96" s="1"/>
       <c r="E96" s="2">
@@ -2686,10 +2686,10 @@
         <v>1</v>
       </c>
       <c r="C97" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D97" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>146</v>
       </c>
       <c r="E97" s="2">
         <v>0</v>
@@ -2705,10 +2705,10 @@
         <v>2</v>
       </c>
       <c r="C98" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D98" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>148</v>
       </c>
       <c r="E98" s="2">
         <v>0</v>
@@ -2724,10 +2724,10 @@
         <v>1</v>
       </c>
       <c r="C99" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D99" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>150</v>
       </c>
       <c r="E99" s="2">
         <v>0</v>
@@ -2743,10 +2743,10 @@
         <v>1</v>
       </c>
       <c r="C100" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D100" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="D100" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="E100" s="2">
         <v>1</v>
@@ -2762,10 +2762,10 @@
         <v>1</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E101" s="2">
         <v>0</v>
@@ -2781,10 +2781,10 @@
         <v>1</v>
       </c>
       <c r="C102" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D102" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="D102" s="1" t="s">
-        <v>153</v>
       </c>
       <c r="E102" s="2">
         <v>0</v>
@@ -2800,10 +2800,10 @@
         <v>1</v>
       </c>
       <c r="C103" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D103" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>153</v>
       </c>
       <c r="E103" s="2">
         <v>0</v>
@@ -2819,10 +2819,10 @@
         <v>1</v>
       </c>
       <c r="C104" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D104" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="D104" s="1" t="s">
-        <v>155</v>
       </c>
       <c r="E104" s="2">
         <v>0</v>
@@ -2838,7 +2838,7 @@
         <v>1</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D105" s="1"/>
       <c r="E105" s="2">
@@ -2855,10 +2855,10 @@
         <v>1</v>
       </c>
       <c r="C106" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D106" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="D106" s="1" t="s">
-        <v>158</v>
       </c>
       <c r="E106" s="2">
         <v>0</v>
@@ -2874,10 +2874,10 @@
         <v>1</v>
       </c>
       <c r="C107" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D107" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="D107" s="1" t="s">
-        <v>160</v>
       </c>
       <c r="E107" s="2">
         <v>0</v>
@@ -2893,10 +2893,10 @@
         <v>2</v>
       </c>
       <c r="C108" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D108" s="1" t="s">
         <v>161</v>
-      </c>
-      <c r="D108" s="1" t="s">
-        <v>162</v>
       </c>
       <c r="E108" s="2">
         <v>0</v>
@@ -2912,10 +2912,10 @@
         <v>1</v>
       </c>
       <c r="C109" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D109" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="D109" s="1" t="s">
-        <v>164</v>
       </c>
       <c r="E109" s="2">
         <v>0</v>
@@ -2931,10 +2931,10 @@
         <v>1</v>
       </c>
       <c r="C110" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D110" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="D110" s="1" t="s">
-        <v>164</v>
       </c>
       <c r="E110" s="2">
         <v>0</v>
@@ -2950,10 +2950,10 @@
         <v>1</v>
       </c>
       <c r="C111" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D111" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="D111" s="1" t="s">
-        <v>166</v>
       </c>
       <c r="E111" s="2">
         <v>0</v>
@@ -2969,10 +2969,10 @@
         <v>1</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E112" s="2">
         <v>0</v>
@@ -2988,10 +2988,10 @@
         <v>1</v>
       </c>
       <c r="C113" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D113" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="D113" s="1" t="s">
-        <v>169</v>
       </c>
       <c r="E113" s="2">
         <v>0</v>
@@ -3007,10 +3007,10 @@
         <v>2</v>
       </c>
       <c r="C114" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D114" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="D114" s="1" t="s">
-        <v>171</v>
       </c>
       <c r="E114" s="2">
         <v>0</v>
@@ -3026,10 +3026,10 @@
         <v>1</v>
       </c>
       <c r="C115" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D115" s="1" t="s">
         <v>172</v>
-      </c>
-      <c r="D115" s="1" t="s">
-        <v>173</v>
       </c>
       <c r="E115" s="2">
         <v>0</v>
@@ -3045,10 +3045,10 @@
         <v>2</v>
       </c>
       <c r="C116" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D116" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="D116" s="1" t="s">
-        <v>175</v>
       </c>
       <c r="E116" s="2">
         <v>0</v>
@@ -3064,10 +3064,10 @@
         <v>1</v>
       </c>
       <c r="C117" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D117" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="D117" s="1" t="s">
-        <v>177</v>
       </c>
       <c r="E117" s="2">
         <v>0</v>
@@ -3083,10 +3083,10 @@
         <v>1</v>
       </c>
       <c r="C118" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D118" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="D118" s="1" t="s">
-        <v>179</v>
       </c>
       <c r="E118" s="2">
         <v>0</v>
@@ -3102,10 +3102,10 @@
         <v>1</v>
       </c>
       <c r="C119" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D119" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="D119" s="1" t="s">
-        <v>153</v>
       </c>
       <c r="E119" s="2">
         <v>0</v>
@@ -3121,10 +3121,10 @@
         <v>1</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E120" s="2">
         <v>0</v>
@@ -3140,10 +3140,10 @@
         <v>1</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E121" s="2">
         <v>0</v>
@@ -3159,10 +3159,10 @@
         <v>1</v>
       </c>
       <c r="C122" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D122" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="D122" s="1" t="s">
-        <v>182</v>
       </c>
       <c r="E122" s="2">
         <v>0</v>
@@ -3178,7 +3178,7 @@
         <v>2</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D123" s="1"/>
       <c r="E123" s="2">
@@ -3195,10 +3195,10 @@
         <v>3</v>
       </c>
       <c r="C124" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D124" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="D124" s="1" t="s">
-        <v>185</v>
       </c>
       <c r="E124" s="2">
         <v>0</v>
@@ -3214,10 +3214,10 @@
         <v>1</v>
       </c>
       <c r="C125" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D125" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="D125" s="1" t="s">
-        <v>187</v>
       </c>
       <c r="E125" s="2">
         <v>0</v>
@@ -3233,10 +3233,10 @@
         <v>1</v>
       </c>
       <c r="C126" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D126" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="D126" s="1" t="s">
-        <v>189</v>
       </c>
       <c r="E126" s="2">
         <v>0</v>

</xml_diff>